<commit_message>
Progress improving wheat model
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/Observations/ABlock99_00_BiomassEarly.xlsx
+++ b/Prototypes/Barley/Observations/ABlock99_00_BiomassEarly.xlsx
@@ -414,11 +414,12 @@
   <dimension ref="A1:F189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F189"/>
+      <selection activeCell="D9" sqref="D9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -592,15 +593,6 @@
       <c r="C9">
         <v>1003.334725</v>
       </c>
-      <c r="D9">
-        <v>51.9412304943245</v>
-      </c>
-      <c r="E9">
-        <v>3.1190088504533966</v>
-      </c>
-      <c r="F9">
-        <v>13.263747579594238</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -892,15 +884,6 @@
       <c r="C24">
         <v>313.97372500000006</v>
       </c>
-      <c r="D24">
-        <v>290.77536702620614</v>
-      </c>
-      <c r="E24">
-        <v>0.44179514445145979</v>
-      </c>
-      <c r="F24">
-        <v>20.670619439503358</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -932,15 +915,6 @@
       <c r="C26">
         <v>1237.5281874999998</v>
       </c>
-      <c r="D26">
-        <v>51.497687350676088</v>
-      </c>
-      <c r="E26">
-        <v>4.4379992984715049</v>
-      </c>
-      <c r="F26">
-        <v>13.012658694211471</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1252,15 +1226,6 @@
       <c r="C42">
         <v>355.91514999999998</v>
       </c>
-      <c r="D42">
-        <v>332.38836496141522</v>
-      </c>
-      <c r="E42">
-        <v>0.50584554817218408</v>
-      </c>
-      <c r="F42">
-        <v>21.289159204632703</v>
-      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1292,15 +1257,6 @@
       <c r="C44">
         <v>1172.2527375000002</v>
       </c>
-      <c r="D44">
-        <v>119.18371210638161</v>
-      </c>
-      <c r="E44">
-        <v>4.0674257423775977</v>
-      </c>
-      <c r="F44">
-        <v>26.477302171706441</v>
-      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1612,15 +1568,6 @@
       <c r="C60">
         <v>489.56846249999995</v>
       </c>
-      <c r="D60">
-        <v>442.58444217152368</v>
-      </c>
-      <c r="E60">
-        <v>0.88288512123631313</v>
-      </c>
-      <c r="F60">
-        <v>44.551511255638196</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1652,15 +1599,6 @@
       <c r="C62">
         <v>1164.3703624999998</v>
       </c>
-      <c r="D62">
-        <v>154.41354869769941</v>
-      </c>
-      <c r="E62">
-        <v>4.3684773855284824</v>
-      </c>
-      <c r="F62">
-        <v>42.112261907800296</v>
-      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -1952,15 +1890,6 @@
       <c r="C77">
         <v>343.56736249999994</v>
       </c>
-      <c r="D77">
-        <v>313.6354762914263</v>
-      </c>
-      <c r="E77">
-        <v>0.53430528618569462</v>
-      </c>
-      <c r="F77">
-        <v>28.202658594295809</v>
-      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -1992,15 +1921,6 @@
       <c r="C79">
         <v>911.48787499999992</v>
       </c>
-      <c r="D79">
-        <v>64.91337307477832</v>
-      </c>
-      <c r="E79">
-        <v>2.7508789697397682</v>
-      </c>
-      <c r="F79">
-        <v>19.906986535342739</v>
-      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -2232,15 +2152,6 @@
       <c r="C91">
         <v>118.33930000000001</v>
       </c>
-      <c r="D91">
-        <v>117.84928730823169</v>
-      </c>
-      <c r="E91">
-        <v>8.2069837178877572E-2</v>
-      </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -2252,15 +2163,6 @@
       <c r="C92">
         <v>387.10652499999998</v>
       </c>
-      <c r="D92">
-        <v>373.33930551130317</v>
-      </c>
-      <c r="E92">
-        <v>0.78146017878709051</v>
-      </c>
-      <c r="F92">
-        <v>9.9910001166077045</v>
-      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
@@ -2432,15 +2334,6 @@
       <c r="C101">
         <v>125.58764999999998</v>
       </c>
-      <c r="D101">
-        <v>125.02128141077091</v>
-      </c>
-      <c r="E101">
-        <v>9.4523075333333373E-2</v>
-      </c>
-      <c r="F101">
-        <v>0.14904901613816537</v>
-      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
@@ -2452,15 +2345,6 @@
       <c r="C102">
         <v>385.1279925</v>
       </c>
-      <c r="D102">
-        <v>366.75762727912115</v>
-      </c>
-      <c r="E102">
-        <v>0.83461281349157501</v>
-      </c>
-      <c r="F102">
-        <v>15.368082626661137</v>
-      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
@@ -2632,15 +2516,6 @@
       <c r="C111">
         <v>209.18317499999998</v>
       </c>
-      <c r="D111">
-        <v>204.23224421087426</v>
-      </c>
-      <c r="E111">
-        <v>0.17429360893318807</v>
-      </c>
-      <c r="F111">
-        <v>4.4627481932289754</v>
-      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -2652,15 +2527,6 @@
       <c r="C112">
         <v>485.85652874999994</v>
       </c>
-      <c r="D112">
-        <v>434.77080696063723</v>
-      </c>
-      <c r="E112">
-        <v>1.1217843834519057</v>
-      </c>
-      <c r="F112">
-        <v>48.318610458859517</v>
-      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
@@ -2832,15 +2698,6 @@
       <c r="C121">
         <v>210.51087500000003</v>
       </c>
-      <c r="D121">
-        <v>205.10442473492674</v>
-      </c>
-      <c r="E121">
-        <v>0.19168639731316109</v>
-      </c>
-      <c r="F121">
-        <v>4.8818819104112219</v>
-      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -2852,15 +2709,6 @@
       <c r="C122">
         <v>593.14142499999991</v>
       </c>
-      <c r="D122">
-        <v>538.02065708978898</v>
-      </c>
-      <c r="E122">
-        <v>1.33193994883574</v>
-      </c>
-      <c r="F122">
-        <v>51.209084024787153</v>
-      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3032,15 +2880,6 @@
       <c r="C131">
         <v>120.445425</v>
       </c>
-      <c r="D131">
-        <v>119.94981162782128</v>
-      </c>
-      <c r="E131">
-        <v>8.7034035778955077E-2</v>
-      </c>
-      <c r="F131">
-        <v>0</v>
-      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
@@ -3051,15 +2890,6 @@
       </c>
       <c r="C132">
         <v>370.30987500000003</v>
-      </c>
-      <c r="D132">
-        <v>344.34467145449003</v>
-      </c>
-      <c r="E132">
-        <v>0.72998771189224554</v>
-      </c>
-      <c r="F132">
-        <v>22.433657404054394</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>